<commit_message>
change log output 2018-3-27-14-27:00
</commit_message>
<xml_diff>
--- a/mypjt/dataFiles/GBP.xlsx
+++ b/mypjt/dataFiles/GBP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>货币名称</t>
   </si>
@@ -62,6 +62,96 @@
   </si>
   <si>
     <t>81.1770</t>
+  </si>
+  <si>
+    <t>8.9071</t>
+  </si>
+  <si>
+    <t>2018-03-27 13:53:00</t>
+  </si>
+  <si>
+    <t>150.3320</t>
+  </si>
+  <si>
+    <t>1.1431</t>
+  </si>
+  <si>
+    <t>1.4229</t>
+  </si>
+  <si>
+    <t>81.2500</t>
+  </si>
+  <si>
+    <t>8.9073</t>
+  </si>
+  <si>
+    <t>2018-03-27 13:55:00</t>
+  </si>
+  <si>
+    <t>150.3110</t>
+  </si>
+  <si>
+    <t>1.1430</t>
+  </si>
+  <si>
+    <t>81.2550</t>
+  </si>
+  <si>
+    <t>2018-03-27 13:58:00</t>
+  </si>
+  <si>
+    <t>150.2750</t>
+  </si>
+  <si>
+    <t>1.4230</t>
+  </si>
+  <si>
+    <t>81.3280</t>
+  </si>
+  <si>
+    <t>8.9017</t>
+  </si>
+  <si>
+    <t>2018-03-27 14:16:00</t>
+  </si>
+  <si>
+    <t>150.2460</t>
+  </si>
+  <si>
+    <t>1.4226</t>
+  </si>
+  <si>
+    <t>81.2990</t>
+  </si>
+  <si>
+    <t>2018-03-27 14:19:00</t>
+  </si>
+  <si>
+    <t>150.2630</t>
+  </si>
+  <si>
+    <t>1.1426</t>
+  </si>
+  <si>
+    <t>1.4232</t>
+  </si>
+  <si>
+    <t>81.3000</t>
+  </si>
+  <si>
+    <t>8.9036</t>
+  </si>
+  <si>
+    <t>2018-03-27 14:25:00</t>
+  </si>
+  <si>
+    <t>150.2410</t>
+  </si>
+  <si>
+    <t>1.1427</t>
+  </si>
+  <si>
+    <t>81.2340</t>
   </si>
 </sst>
 </file>
@@ -397,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +559,336 @@
       </c>
       <c r="C6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +902,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +924,54 @@
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -517,7 +985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +1007,54 @@
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +1068,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,6 +1090,54 @@
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -587,7 +1151,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +1173,54 @@
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +1234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +1258,54 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>